<commit_message>
BugFix 1. fixed assigning people to tickets in certain column
</commit_message>
<xml_diff>
--- a/sprints/Sprint4/sprint4_Blacklog.xlsx
+++ b/sprints/Sprint4/sprint4_Blacklog.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jh00291\Documents\GitHub\CapstoneProjectGroup7\sprints\Sprint4\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\drivera3\source\repos\CapstoneProjectGroup7\sprints\Sprint4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3A3208B-B8B1-465F-9D67-C5115875E96C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7827DC50-9026-43FE-9309-D6B88E52FE6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1510" windowWidth="28800" windowHeight="15460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="20295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
   <si>
     <t>Related User Story</t>
   </si>
@@ -87,6 +87,9 @@
   </si>
   <si>
     <t>&lt;optional&gt; Implement post comments  (Desktop)</t>
+  </si>
+  <si>
+    <t>Daniel</t>
   </si>
 </sst>
 </file>
@@ -1345,18 +1348,18 @@
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="59.453125" customWidth="1"/>
-    <col min="2" max="2" width="23.7265625" customWidth="1"/>
-    <col min="3" max="3" width="14.1796875" customWidth="1"/>
-    <col min="4" max="4" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="59.42578125" customWidth="1"/>
+    <col min="2" max="2" width="23.7109375" customWidth="1"/>
+    <col min="3" max="3" width="14.140625" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -1371,7 +1374,7 @@
       <c r="F1" s="7"/>
       <c r="G1" s="7"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="8"/>
       <c r="B2" s="5" t="s">
         <v>5</v>
@@ -1384,11 +1387,13 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="6"/>
+      <c r="B3" s="6" t="s">
+        <v>17</v>
+      </c>
       <c r="C3" s="6">
         <v>3</v>
       </c>
@@ -1399,11 +1404,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="6"/>
+      <c r="B4" s="6" t="s">
+        <v>17</v>
+      </c>
       <c r="C4" s="6">
         <v>3</v>
       </c>
@@ -1414,11 +1421,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="6"/>
+      <c r="B5" s="6" t="s">
+        <v>17</v>
+      </c>
       <c r="C5" s="6">
         <v>1</v>
       </c>
@@ -1429,11 +1438,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="6"/>
+      <c r="B6" s="6" t="s">
+        <v>17</v>
+      </c>
       <c r="C6" s="6">
         <v>2</v>
       </c>
@@ -1444,7 +1455,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>12</v>
       </c>
@@ -1461,7 +1472,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>13</v>
       </c>
@@ -1478,7 +1489,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>14</v>
       </c>
@@ -1493,7 +1504,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>15</v>
       </c>
@@ -1508,7 +1519,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>11</v>
       </c>
@@ -1523,7 +1534,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>16</v>
       </c>
@@ -1538,14 +1549,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="6"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C14" s="3">
         <f>SUM(C3:C13)</f>
         <v>22</v>

</xml_diff>